<commit_message>
:sparkles: :construction: update HyperparamTuner.train_test_return nyní lze extrahovat predikované hodnoty y_test
</commit_message>
<xml_diff>
--- a/project_resources/optuna/optuna_rmsds.xlsx
+++ b/project_resources/optuna/optuna_rmsds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Downloads\optuna_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Documents\datacytochromy\project_resources\optuna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2185770-41CA-4B27-8AA0-EFF77F4213CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D13F91-D775-4446-AB87-97FB14E5CAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{3A496B5D-D67D-4DA1-B5CC-3FC2C604CE09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A496B5D-D67D-4DA1-B5CC-3FC2C604CE09}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="34">
   <si>
     <t>random</t>
   </si>
@@ -71,15 +71,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>3A4: 70 molekul</t>
-  </si>
-  <si>
-    <t>RLM: 2530 molekul</t>
-  </si>
-  <si>
-    <t>HLC: 189 molekul</t>
-  </si>
-  <si>
     <t>OPTUNA</t>
   </si>
   <si>
@@ -120,6 +111,33 @@
   </si>
   <si>
     <t>JAZZY FEATURES</t>
+  </si>
+  <si>
+    <t>n_trials = 50</t>
+  </si>
+  <si>
+    <t>n_trials = 200</t>
+  </si>
+  <si>
+    <t>runtime … 4 hrs</t>
+  </si>
+  <si>
+    <t>HLC: 189 mols</t>
+  </si>
+  <si>
+    <t>RLM: 2530 mols</t>
+  </si>
+  <si>
+    <t>3A4: 70 mols</t>
+  </si>
+  <si>
+    <t>HLC-GB</t>
+  </si>
+  <si>
+    <t>Lower rmsd with scikit-learn</t>
+  </si>
+  <si>
+    <t>Lower rmsd with Optuna</t>
   </si>
 </sst>
 </file>
@@ -129,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,13 +156,34 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,12 +198,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -479,59 +529,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A39277-9E89-402B-A72C-D043DAA2EEA0}">
-  <dimension ref="B2:AC31"/>
+  <dimension ref="B2:AD57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB34" sqref="AB34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="P3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="X6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -562,38 +618,38 @@
       <c r="N8" t="s">
         <v>8</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>4</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>5</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>6</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>7</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>8</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>4</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>5</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>6</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>7</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -630,44 +686,44 @@
       <c r="N9" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>1</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>1.361</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>1.3979999999999999</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <v>1.0629999999999999</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>1.1180000000000001</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <v>2.89</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>1</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <v>1.363</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AA9" s="2">
         <v>1.375</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AB9" s="2">
         <v>1.0149999999999999</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AC9" s="2">
         <v>1.121</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AD9" s="2">
         <v>2.36</v>
       </c>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -704,49 +760,49 @@
       <c r="N10" s="2">
         <v>1.0349999999999999</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>2</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>1.054</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>1.1080000000000001</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>0.99199999999999999</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>0.98599999999999999</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>1.0389999999999999</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>2</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Z10" s="2">
         <v>1.06</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AA10" s="2">
         <v>1.1100000000000001</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AB10" s="2">
         <v>0.999</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AC10" s="2">
         <v>0.99299999999999999</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AD10" s="2">
         <v>1.008</v>
       </c>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2">
         <v>0.58599999999999997</v>
@@ -764,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K11" s="2">
         <v>0.55000000000000004</v>
@@ -778,168 +834,168 @@
       <c r="N11" s="2">
         <v>1.0840000000000001</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="2">
+      <c r="S11" s="2">
         <v>0.60099999999999998</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>0.86499999999999999</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>0.623</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="2">
         <v>0.58599999999999997</v>
       </c>
-      <c r="V11" s="2">
+      <c r="W11" s="2">
         <v>1.6819999999999999</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>3</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Z11" s="2">
         <v>0.79100000000000004</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>0.46300000000000002</v>
       </c>
       <c r="AA11" s="2">
         <v>0.46300000000000002</v>
       </c>
       <c r="AB11" s="2">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="AC11" s="2">
         <v>0.44900000000000001</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="AD11" s="2">
         <v>1.631</v>
       </c>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2">
         <f>MIN(C9:G9)</f>
         <v>1.125</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L13" s="2">
         <f>MIN(J9:N9)</f>
         <v>1.1359999999999999</v>
       </c>
-      <c r="R13" t="s">
-        <v>25</v>
-      </c>
       <c r="S13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13" t="s">
         <v>1</v>
       </c>
-      <c r="T13" s="2">
-        <f>MIN(R9:V9)</f>
+      <c r="U13" s="2">
+        <f>MIN(S9:W9)</f>
         <v>1.0629999999999999</v>
       </c>
-      <c r="Y13" t="s">
-        <v>25</v>
-      </c>
       <c r="Z13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA13" t="s">
         <v>1</v>
       </c>
-      <c r="AA13" s="2">
-        <f>MIN(Y9:AC9)</f>
+      <c r="AB13" s="2">
+        <f>MIN(Z9:AD9)</f>
         <v>1.0149999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2">
         <f>MIN(C10:G10)</f>
         <v>0.95</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L14" s="2">
         <f>MIN(J10:N10)</f>
         <v>0.95899999999999996</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>2</v>
       </c>
-      <c r="T14" s="2">
-        <f>MIN(R10:V10)</f>
+      <c r="U14" s="2">
+        <f>MIN(S10:W10)</f>
         <v>0.98599999999999999</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>2</v>
       </c>
-      <c r="AA14" s="2">
-        <f>MIN(Y10:AC10)</f>
+      <c r="AB14" s="2">
+        <f>MIN(Z10:AD10)</f>
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2">
         <f>MIN(C11:G11)</f>
         <v>0.51800000000000002</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L15" s="2">
         <f>MIN(J11:N11)</f>
         <v>0.44</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>3</v>
       </c>
-      <c r="T15" s="2">
-        <f>MIN(R11:V11)</f>
+      <c r="U15" s="2">
+        <f>MIN(S11:W11)</f>
         <v>0.58599999999999997</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>3</v>
       </c>
-      <c r="AA15" s="2">
-        <f>MIN(Y11:AC11)</f>
+      <c r="AB15" s="2">
+        <f>MIN(Z11:AD11)</f>
         <v>0.44900000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="H16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AB17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -970,38 +1026,38 @@
       <c r="N18" t="s">
         <v>8</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>4</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>5</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>6</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>7</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>8</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>4</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AA18" t="s">
         <v>5</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>6</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AC18" t="s">
         <v>7</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1038,44 +1094,44 @@
       <c r="N19" s="2">
         <v>1.371</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>1</v>
       </c>
-      <c r="R19" s="2">
+      <c r="S19" s="2">
         <v>1.8779999999999999</v>
       </c>
-      <c r="S19" s="2">
+      <c r="T19" s="2">
         <v>1.6830000000000001</v>
       </c>
-      <c r="T19" s="2">
+      <c r="U19" s="2">
         <v>1.3069999999999999</v>
       </c>
-      <c r="U19" s="2">
+      <c r="V19" s="2">
         <v>1.522</v>
       </c>
-      <c r="V19" s="2">
+      <c r="W19" s="2">
         <v>1.677</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>1</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Z19" s="2">
         <v>1.5069999999999999</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="AA19" s="2">
         <v>1.4850000000000001</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AB19" s="2">
         <v>1.421</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="AC19" s="2">
         <v>1.448</v>
       </c>
-      <c r="AC19" s="2">
+      <c r="AD19" s="2">
         <v>1.6539999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1112,44 +1168,44 @@
       <c r="N20" s="2">
         <v>1.3839999999999999</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="2">
+      <c r="S20" s="2">
         <v>0.98299999999999998</v>
       </c>
-      <c r="S20" s="2">
+      <c r="T20" s="2">
         <v>0.96199999999999997</v>
       </c>
-      <c r="T20" s="2">
+      <c r="U20" s="2">
         <v>0.96299999999999997</v>
       </c>
-      <c r="U20" s="2">
+      <c r="V20" s="2">
         <v>0.93700000000000006</v>
       </c>
-      <c r="V20" s="2">
+      <c r="W20" s="2">
         <v>0.995</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>2</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Z20" s="2">
         <v>1.339</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="AA20" s="2">
         <v>1.3440000000000001</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AB20" s="2">
         <v>1.3520000000000001</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AC20" s="2">
         <v>1.3560000000000001</v>
       </c>
-      <c r="AC20" s="2">
+      <c r="AD20" s="2">
         <v>1.38</v>
       </c>
     </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1186,168 +1242,168 @@
       <c r="N21" s="2">
         <v>1.4410000000000001</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>3</v>
       </c>
-      <c r="R21" s="2">
+      <c r="S21" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>0.51500000000000001</v>
       </c>
-      <c r="T21" s="2">
+      <c r="U21" s="2">
         <v>0.51600000000000001</v>
       </c>
-      <c r="U21" s="2">
+      <c r="V21" s="2">
         <v>0.505</v>
       </c>
-      <c r="V21" s="2">
+      <c r="W21" s="2">
         <v>0.92700000000000005</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>3</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Z21" s="2">
         <v>1.284</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="AA21" s="2">
         <v>1.2649999999999999</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AB21" s="2">
         <v>1.2809999999999999</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="AC21" s="2">
         <v>1.2470000000000001</v>
       </c>
-      <c r="AC21" s="2">
+      <c r="AD21" s="2">
         <v>1.4510000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E23" s="2">
         <f>MIN(C19:G19)</f>
         <v>1.3360000000000001</v>
       </c>
       <c r="J23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L23" s="2">
         <f>MIN(J19:N19)</f>
         <v>1.3089999999999999</v>
       </c>
-      <c r="R23" t="s">
-        <v>25</v>
-      </c>
       <c r="S23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" t="s">
         <v>1</v>
       </c>
-      <c r="T23" s="2">
-        <f>MIN(R19:V19)</f>
+      <c r="U23" s="2">
+        <f>MIN(S19:W19)</f>
         <v>1.3069999999999999</v>
       </c>
-      <c r="Y23" t="s">
-        <v>25</v>
-      </c>
       <c r="Z23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA23" t="s">
         <v>1</v>
       </c>
-      <c r="AA23" s="2">
-        <f>MIN(Y19:AC19)</f>
+      <c r="AB23" s="2">
+        <f>MIN(Z19:AD19)</f>
         <v>1.421</v>
       </c>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E24" s="2">
         <f>MIN(C20:G20)</f>
         <v>0.88100000000000001</v>
       </c>
       <c r="K24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L24" s="2">
         <f>MIN(J20:N20)</f>
         <v>1.3420000000000001</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>2</v>
       </c>
-      <c r="T24" s="2">
-        <f>MIN(R20:V20)</f>
+      <c r="U24" s="2">
+        <f>MIN(S20:W20)</f>
         <v>0.93700000000000006</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AA24" t="s">
         <v>2</v>
       </c>
-      <c r="AA24" s="2">
-        <f>MIN(Y20:AC20)</f>
+      <c r="AB24" s="2">
+        <f>MIN(Z20:AD20)</f>
         <v>1.339</v>
       </c>
     </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2">
         <f>MIN(C21:G21)</f>
         <v>0.54400000000000004</v>
       </c>
       <c r="K25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L25" s="2">
         <f>MIN(J21:N21)</f>
         <v>1.2949999999999999</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>3</v>
       </c>
-      <c r="T25" s="2">
-        <f>MIN(R21:V21)</f>
+      <c r="U25" s="2">
+        <f>MIN(S21:W21)</f>
         <v>0.505</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="AA25" t="s">
         <v>3</v>
       </c>
-      <c r="AA25" s="2">
-        <f>MIN(Y21:AC21)</f>
+      <c r="AB25" s="2">
+        <f>MIN(Z21:AD21)</f>
         <v>1.2470000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="H26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>0</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>0</v>
       </c>
-      <c r="AA27" s="1" t="s">
+      <c r="AB27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>4</v>
       </c>
@@ -1378,38 +1434,38 @@
       <c r="N28" t="s">
         <v>8</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>4</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>5</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>6</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>7</v>
       </c>
-      <c r="V28" t="s">
+      <c r="W28" t="s">
         <v>8</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>4</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="AA28" t="s">
         <v>5</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AB28" t="s">
         <v>6</v>
       </c>
-      <c r="AB28" t="s">
+      <c r="AC28" t="s">
         <v>7</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="AD28" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>1</v>
       </c>
@@ -1456,54 +1512,54 @@
         <f t="shared" si="1"/>
         <v>0.22100000000000009</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>1</v>
       </c>
-      <c r="R29" s="2">
-        <f t="shared" ref="R29:V29" si="2">R19-R9</f>
+      <c r="S29" s="2">
+        <f t="shared" ref="S29:W29" si="2">S19-S9</f>
         <v>0.5169999999999999</v>
       </c>
-      <c r="S29" s="2">
+      <c r="T29" s="2">
         <f t="shared" si="2"/>
         <v>0.28500000000000014</v>
       </c>
-      <c r="T29" s="2">
+      <c r="U29" s="2">
         <f t="shared" si="2"/>
         <v>0.24399999999999999</v>
       </c>
-      <c r="U29" s="2">
+      <c r="V29" s="2">
         <f t="shared" si="2"/>
         <v>0.40399999999999991</v>
       </c>
-      <c r="V29" s="2">
+      <c r="W29" s="2">
         <f t="shared" si="2"/>
         <v>-1.2130000000000001</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Y29" t="s">
         <v>1</v>
       </c>
-      <c r="Y29" s="2">
-        <f xml:space="preserve"> Y19-Y9</f>
+      <c r="Z29" s="2">
+        <f xml:space="preserve"> Z19-Z9</f>
         <v>0.14399999999999991</v>
       </c>
-      <c r="Z29" s="2">
-        <f t="shared" ref="Z29:AC29" si="3" xml:space="preserve"> Z19-Z9</f>
+      <c r="AA29" s="2">
+        <f t="shared" ref="AA29:AD29" si="3" xml:space="preserve"> AA19-AA9</f>
         <v>0.1100000000000001</v>
       </c>
-      <c r="AA29" s="2">
+      <c r="AB29" s="2">
         <f t="shared" si="3"/>
         <v>0.40600000000000014</v>
       </c>
-      <c r="AB29" s="2">
+      <c r="AC29" s="2">
         <f t="shared" si="3"/>
         <v>0.32699999999999996</v>
       </c>
-      <c r="AC29" s="2">
+      <c r="AD29" s="2">
         <f t="shared" si="3"/>
         <v>-0.70599999999999996</v>
       </c>
     </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>2</v>
       </c>
@@ -1550,54 +1606,54 @@
         <f t="shared" si="1"/>
         <v>0.34899999999999998</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>2</v>
       </c>
-      <c r="R30" s="2">
-        <f t="shared" ref="R30:V30" si="4">R20-R10</f>
+      <c r="S30" s="2">
+        <f t="shared" ref="S30:W30" si="4">S20-S10</f>
         <v>-7.1000000000000063E-2</v>
       </c>
-      <c r="S30" s="2">
+      <c r="T30" s="2">
         <f t="shared" si="4"/>
         <v>-0.14600000000000013</v>
       </c>
-      <c r="T30" s="2">
+      <c r="U30" s="2">
         <f t="shared" si="4"/>
         <v>-2.9000000000000026E-2</v>
       </c>
-      <c r="U30" s="2">
+      <c r="V30" s="2">
         <f t="shared" si="4"/>
         <v>-4.8999999999999932E-2</v>
       </c>
-      <c r="V30" s="2">
+      <c r="W30" s="2">
         <f t="shared" si="4"/>
         <v>-4.3999999999999928E-2</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Y30" t="s">
         <v>2</v>
       </c>
-      <c r="Y30" s="2">
-        <f t="shared" ref="Y30:AC30" si="5" xml:space="preserve"> Y20-Y10</f>
+      <c r="Z30" s="2">
+        <f t="shared" ref="Z30:AD30" si="5" xml:space="preserve"> Z20-Z10</f>
         <v>0.27899999999999991</v>
       </c>
-      <c r="Z30" s="2">
+      <c r="AA30" s="2">
         <f t="shared" si="5"/>
         <v>0.23399999999999999</v>
       </c>
-      <c r="AA30" s="2">
+      <c r="AB30" s="2">
         <f t="shared" si="5"/>
         <v>0.35300000000000009</v>
       </c>
-      <c r="AB30" s="2">
+      <c r="AC30" s="2">
         <f t="shared" si="5"/>
         <v>0.3630000000000001</v>
       </c>
-      <c r="AC30" s="2">
+      <c r="AD30" s="2">
         <f t="shared" si="5"/>
         <v>0.37199999999999989</v>
       </c>
     </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -1642,53 +1698,940 @@
         <f>N21-N11</f>
         <v>0.35699999999999998</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>3</v>
       </c>
-      <c r="R31" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="S31" s="2">
-        <f>T21-S11</f>
-        <v>-0.34899999999999998</v>
+        <f>S21-S11</f>
+        <v>-4.599999999999993E-2</v>
       </c>
       <c r="T31" s="2">
         <f>U21-T11</f>
-        <v>-0.11799999999999999</v>
+        <v>-0.34899999999999998</v>
       </c>
       <c r="U31" s="2">
         <f>V21-U11</f>
+        <v>-0.11799999999999999</v>
+      </c>
+      <c r="V31" s="2">
+        <f>W21-V11</f>
         <v>0.34100000000000008</v>
       </c>
-      <c r="V31" s="2">
-        <f>V21-V11</f>
+      <c r="W31" s="2">
+        <f>W21-W11</f>
         <v>-0.75499999999999989</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Y31" t="s">
         <v>3</v>
       </c>
-      <c r="Y31" s="2">
-        <f t="shared" ref="Y31:AC31" si="6" xml:space="preserve"> Y21-Y11</f>
+      <c r="Z31" s="2">
+        <f t="shared" ref="Z31:AD31" si="6" xml:space="preserve"> Z21-Z11</f>
         <v>0.49299999999999999</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="AA31" s="2">
         <f t="shared" si="6"/>
         <v>0.80199999999999982</v>
       </c>
-      <c r="AA31" s="2">
+      <c r="AB31" s="2">
         <f t="shared" si="6"/>
         <v>0.81799999999999984</v>
       </c>
-      <c r="AB31" s="2">
+      <c r="AC31" s="2">
         <f t="shared" si="6"/>
         <v>0.79800000000000004</v>
       </c>
-      <c r="AC31" s="2">
+      <c r="AD31" s="2">
         <f t="shared" si="6"/>
         <v>-0.17999999999999994</v>
       </c>
     </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="O34" s="4"/>
+      <c r="P34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q34" s="4"/>
+    </row>
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="O36" s="6"/>
+      <c r="P36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="X39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="H40" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="P41" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+      <c r="X42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44" t="s">
+        <v>7</v>
+      </c>
+      <c r="N44" t="s">
+        <v>8</v>
+      </c>
+      <c r="S44" t="s">
+        <v>4</v>
+      </c>
+      <c r="T44" t="s">
+        <v>5</v>
+      </c>
+      <c r="U44" t="s">
+        <v>6</v>
+      </c>
+      <c r="V44" t="s">
+        <v>7</v>
+      </c>
+      <c r="W44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1.3640000000000001</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1.216</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1.103</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2">
+        <v>1.3640000000000001</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L45" s="2">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="M45" s="2">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="N45" s="2">
+        <v>1.1339999999999999</v>
+      </c>
+      <c r="R45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S45" s="2">
+        <v>1.359</v>
+      </c>
+      <c r="T45" s="2">
+        <v>1.3560000000000001</v>
+      </c>
+      <c r="U45" s="2">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="V45" s="2">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="W45" s="2">
+        <v>2.9550000000000001</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="2">
+        <v>1.367</v>
+      </c>
+      <c r="AA45" s="2">
+        <v>1.349</v>
+      </c>
+      <c r="AB45" s="2">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AC45" s="2">
+        <v>1.087</v>
+      </c>
+      <c r="AD45" s="2">
+        <v>2.4369999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1.008</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="I46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J46" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K46" s="2">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="L46" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="M46" s="2">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="N46" s="2">
+        <v>1.038</v>
+      </c>
+      <c r="R46" t="s">
+        <v>2</v>
+      </c>
+      <c r="S46" s="2">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="T46" s="2">
+        <v>1.1080000000000001</v>
+      </c>
+      <c r="U46" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="V46" s="2">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="W46" s="2">
+        <v>1.032</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z46" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AB46" s="2">
+        <v>0.999</v>
+      </c>
+      <c r="AC46" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AD46" s="2">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.623</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.996</v>
+      </c>
+      <c r="I47" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="L47" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="M47" s="2">
+        <v>0.443</v>
+      </c>
+      <c r="N47" s="2">
+        <v>1.075</v>
+      </c>
+      <c r="R47" t="s">
+        <v>3</v>
+      </c>
+      <c r="S47" s="2">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="T47" s="2">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="U47" s="2">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="V47" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="W47" s="2">
+        <v>1.2569999999999999</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z47" s="2">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="AB47" s="2">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="AC47" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="AD47" s="2">
+        <v>1.052</v>
+      </c>
+    </row>
+    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="2">
+        <f>MIN(C45:G45)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J49" t="s">
+        <v>22</v>
+      </c>
+      <c r="K49" t="s">
+        <v>17</v>
+      </c>
+      <c r="L49" s="2">
+        <f>MIN(J45:N45)</f>
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="S49" t="s">
+        <v>22</v>
+      </c>
+      <c r="T49" t="s">
+        <v>19</v>
+      </c>
+      <c r="U49" s="2">
+        <f>MIN(S45:W45)</f>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB49" s="2">
+        <f>MIN(Z45:AD45)</f>
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" ref="E50:E51" si="7">MIN(C46:G46)</f>
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="K50" t="s">
+        <v>15</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" ref="L50:L51" si="8">MIN(J46:N46)</f>
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="T50" t="s">
+        <v>15</v>
+      </c>
+      <c r="U50" s="2">
+        <f t="shared" ref="U50:U51" si="9">MIN(S46:W46)</f>
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB50" s="2">
+        <f t="shared" ref="AB50:AB51" si="10">MIN(Z46:AD46)</f>
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51</v>
+      </c>
+      <c r="K51" t="s">
+        <v>16</v>
+      </c>
+      <c r="L51" s="2">
+        <f t="shared" si="8"/>
+        <v>0.443</v>
+      </c>
+      <c r="T51" t="s">
+        <v>16</v>
+      </c>
+      <c r="U51" s="2">
+        <f t="shared" si="9"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB51" s="2">
+        <f t="shared" si="10"/>
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="H52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>0</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U53" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" t="s">
+        <v>4</v>
+      </c>
+      <c r="K54" t="s">
+        <v>5</v>
+      </c>
+      <c r="L54" t="s">
+        <v>6</v>
+      </c>
+      <c r="M54" t="s">
+        <v>7</v>
+      </c>
+      <c r="N54" t="s">
+        <v>8</v>
+      </c>
+      <c r="S54" t="s">
+        <v>4</v>
+      </c>
+      <c r="T54" t="s">
+        <v>5</v>
+      </c>
+      <c r="U54" t="s">
+        <v>6</v>
+      </c>
+      <c r="V54" t="s">
+        <v>7</v>
+      </c>
+      <c r="W54" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2">
+        <f>C19-C45</f>
+        <v>0.44599999999999995</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" ref="D55:G55" si="11">D19-D45</f>
+        <v>0.43899999999999983</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="11"/>
+        <v>0.15700000000000003</v>
+      </c>
+      <c r="F55" s="2">
+        <f t="shared" si="11"/>
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="11"/>
+        <v>0.57200000000000006</v>
+      </c>
+      <c r="I55" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2">
+        <f>J19-J45</f>
+        <v>0.39299999999999979</v>
+      </c>
+      <c r="K55" s="2">
+        <f t="shared" ref="K55:N55" si="12">K19-K45</f>
+        <v>3.6999999999999922E-2</v>
+      </c>
+      <c r="L55" s="2">
+        <f t="shared" si="12"/>
+        <v>0.17100000000000004</v>
+      </c>
+      <c r="M55" s="2">
+        <f t="shared" si="12"/>
+        <v>0.29900000000000015</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" si="12"/>
+        <v>0.2370000000000001</v>
+      </c>
+      <c r="R55" t="s">
+        <v>1</v>
+      </c>
+      <c r="S55" s="2">
+        <f>S19-S45</f>
+        <v>0.51899999999999991</v>
+      </c>
+      <c r="T55" s="2">
+        <f t="shared" ref="T55:W55" si="13">T19-T45</f>
+        <v>0.32699999999999996</v>
+      </c>
+      <c r="U55" s="2">
+        <f t="shared" si="13"/>
+        <v>0.28200000000000003</v>
+      </c>
+      <c r="V55" s="2">
+        <f t="shared" si="13"/>
+        <v>0.41599999999999993</v>
+      </c>
+      <c r="W55" s="2">
+        <f t="shared" si="13"/>
+        <v>-1.278</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="2">
+        <f>Z19-Z45</f>
+        <v>0.1399999999999999</v>
+      </c>
+      <c r="AA55" s="2">
+        <f t="shared" ref="AA55:AD55" si="14">AA19-AA45</f>
+        <v>0.13600000000000012</v>
+      </c>
+      <c r="AB55" s="2">
+        <f t="shared" si="14"/>
+        <v>0.44200000000000006</v>
+      </c>
+      <c r="AC55" s="2">
+        <f t="shared" si="14"/>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="AD55" s="2">
+        <f t="shared" si="14"/>
+        <v>-0.78299999999999992</v>
+      </c>
+    </row>
+    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" ref="C56:G56" si="15">C20-C46</f>
+        <v>-0.14200000000000013</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="15"/>
+        <v>-0.127</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="15"/>
+        <v>-8.0999999999999961E-2</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="15"/>
+        <v>-4.7999999999999932E-2</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="15"/>
+        <v>-9.2999999999999972E-2</v>
+      </c>
+      <c r="I56" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" ref="J56:N56" si="16">J20-J46</f>
+        <v>0.2739999999999998</v>
+      </c>
+      <c r="K56" s="2">
+        <f t="shared" si="16"/>
+        <v>0.32700000000000018</v>
+      </c>
+      <c r="L56" s="2">
+        <f t="shared" si="16"/>
+        <v>0.38200000000000012</v>
+      </c>
+      <c r="M56" s="2">
+        <f t="shared" si="16"/>
+        <v>0.44099999999999995</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="16"/>
+        <v>0.34599999999999986</v>
+      </c>
+      <c r="R56" t="s">
+        <v>2</v>
+      </c>
+      <c r="S56" s="2">
+        <f t="shared" ref="S56:W56" si="17">S20-S46</f>
+        <v>-6.9999999999999951E-2</v>
+      </c>
+      <c r="T56" s="2">
+        <f t="shared" si="17"/>
+        <v>-0.14600000000000013</v>
+      </c>
+      <c r="U56" s="2">
+        <f t="shared" si="17"/>
+        <v>-2.7000000000000024E-2</v>
+      </c>
+      <c r="V56" s="2">
+        <f t="shared" si="17"/>
+        <v>-4.9999999999999933E-2</v>
+      </c>
+      <c r="W56" s="2">
+        <f t="shared" si="17"/>
+        <v>-3.7000000000000033E-2</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z56" s="2">
+        <f t="shared" ref="Z56:AD56" si="18">Z20-Z46</f>
+        <v>0.27899999999999991</v>
+      </c>
+      <c r="AA56" s="2">
+        <f t="shared" si="18"/>
+        <v>0.23399999999999999</v>
+      </c>
+      <c r="AB56" s="2">
+        <f t="shared" si="18"/>
+        <v>0.35300000000000009</v>
+      </c>
+      <c r="AC56" s="2">
+        <f t="shared" si="18"/>
+        <v>0.3630000000000001</v>
+      </c>
+      <c r="AD56" s="2">
+        <f t="shared" si="18"/>
+        <v>0.37399999999999989</v>
+      </c>
+    </row>
+    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" ref="C57:G57" si="19">C21-C47</f>
+        <v>-9.000000000000008E-3</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="19"/>
+        <v>-2.200000000000002E-2</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="19"/>
+        <v>4.8000000000000043E-2</v>
+      </c>
+      <c r="F57" s="2">
+        <f t="shared" si="19"/>
+        <v>2.4000000000000021E-2</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.39300000000000002</v>
+      </c>
+      <c r="I57" t="s">
+        <v>3</v>
+      </c>
+      <c r="J57" s="2">
+        <f t="shared" ref="J57:N57" si="20">J21-J47</f>
+        <v>0.80099999999999993</v>
+      </c>
+      <c r="K57" s="2">
+        <f t="shared" si="20"/>
+        <v>0.75399999999999989</v>
+      </c>
+      <c r="L57" s="2">
+        <f t="shared" si="20"/>
+        <v>0.87599999999999989</v>
+      </c>
+      <c r="M57" s="2">
+        <f t="shared" si="20"/>
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="20"/>
+        <v>0.3660000000000001</v>
+      </c>
+      <c r="R57" t="s">
+        <v>3</v>
+      </c>
+      <c r="S57" s="2">
+        <f t="shared" ref="S57:W57" si="21">S21-S47</f>
+        <v>-4.599999999999993E-2</v>
+      </c>
+      <c r="T57" s="2">
+        <f t="shared" si="21"/>
+        <v>-0.34899999999999998</v>
+      </c>
+      <c r="U57" s="2">
+        <f t="shared" si="21"/>
+        <v>-9.1999999999999971E-2</v>
+      </c>
+      <c r="V57" s="2">
+        <f t="shared" si="21"/>
+        <v>-7.4999999999999956E-2</v>
+      </c>
+      <c r="W57" s="2">
+        <f t="shared" si="21"/>
+        <v>-0.32999999999999985</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z57" s="2">
+        <f t="shared" ref="Z57:AD57" si="22">Z21-Z47</f>
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="AA57" s="2">
+        <f t="shared" si="22"/>
+        <v>0.47499999999999987</v>
+      </c>
+      <c r="AB57" s="2">
+        <f t="shared" si="22"/>
+        <v>0.82199999999999984</v>
+      </c>
+      <c r="AC57" s="2">
+        <f t="shared" si="22"/>
+        <v>0.80900000000000016</v>
+      </c>
+      <c r="AD57" s="2">
+        <f t="shared" si="22"/>
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C55:G57">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J55:N57">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S55:W57">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z55:AD57">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z29:AD31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S29:W31">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:N31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29:G31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>